<commit_message>
fix descriptions and IG building
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-KBV-PR-Base-Practitioner.xlsx
+++ b/output/StructureDefinition-KBV-PR-Base-Practitioner.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-26T13:37:22+01:00</t>
+    <t>2025-04-15T09:45:28+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Dieses Profil bildet eine behandelnde Person ab.</t>
+    <t>The profile of the UTN Practitoner</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
fixing minor errors for IG
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-KBV-PR-Base-Practitioner.xlsx
+++ b/output/StructureDefinition-KBV-PR-Base-Practitioner.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-16T13:27:07+02:00</t>
+    <t>2025-05-10T09:33:17+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2465,17 +2465,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="68.8671875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="45.796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="21.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="59.40625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="39.50390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="18.375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="33.17578125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="83.39453125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="71.9375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -2484,21 +2484,21 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="41.3125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="105.5078125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.1171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="35.63671875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="91.01171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="50.99609375" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="34.578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="28.8359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
   </cols>
   <sheetData>

</xml_diff>